<commit_message>
Finalized STY and Template STY
</commit_message>
<xml_diff>
--- a/TEMPLATE_STY.xlsx
+++ b/TEMPLATE_STY.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\GARRY\Desktop\NEW BOND AUTOMATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMMING\Python\excelProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F79AF9-B5C3-4125-9EFD-7BBD8AB5FCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STY" sheetId="1" r:id="rId1"/>
@@ -18,29 +19,27 @@
     <sheet name="INDBK" sheetId="4" r:id="rId4"/>
     <sheet name="OR" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
-  <si>
-    <t>G(16)-1976921</t>
-  </si>
-  <si>
-    <t>DAWN ENGINEERING CONSTRUCTION &amp; SUPPLY-ANTIPOLO, BAGAMANOC, CATANDUANES</t>
-  </si>
-  <si>
-    <t>NIA-ALBAYCATANDUANES IRR. MAGMT. OFFICE</t>
-  </si>
-  <si>
-    <t>TWO HUNDRED THIRTY FOUR</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>IN LIEU OF TEN (10%) RETENTION  FOR THE PROJECT:</t>
-  </si>
-  <si>
-    <t>REPAIR/RESTORATION OF LIBJO CIS, BATO, CATANDUANES CAT RREIS-009-23INF</t>
   </si>
   <si>
     <t>THIS BOND IS CALLABLE ON DEMAND   PURSUANT TO THE PROVISIONS OF THE  I.R.R. OF R.A 9184 .</t>
@@ -49,16 +48,7 @@
     <t>PROVIDED HOWEVER, that the maximum limit of the surety hereunder shall in no case exceed the sum of PESOS:</t>
   </si>
   <si>
-    <t>TWO HUNDRED THIRTY FOUR THOUSAND TWO HUNDRED  PESOS ONLY</t>
-  </si>
-  <si>
-    <t>(Php234,200.00; Philippine Currencies)</t>
-  </si>
-  <si>
     <t>VIRAC, CATANDUANES</t>
-  </si>
-  <si>
-    <t>ENGR. CHARLON G. CAADLAWON</t>
   </si>
   <si>
     <t>GEMMA T. SARMIENTO</t>
@@ -73,94 +63,118 @@
     <t>Legazpi City</t>
   </si>
   <si>
-    <t>ANTIPOLO, BAGAMANOC, CATANDUANES</t>
-  </si>
-  <si>
-    <t>DAWN ENGINEERING CONSTRUCTION &amp; SUPPLY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TWO HUNDRED THIRTY FOUR THOUSAND TWO HUNDRED  </t>
-  </si>
-  <si>
-    <t>PESOS ONLY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOUR THOUSAND TWO HUNDRED TWENTY SIX  </t>
-  </si>
-  <si>
-    <t>AND 410/100 ONLY</t>
-  </si>
-  <si>
     <t>ONE (1) YEAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                     THOUSAND TWO HUNDRED  PESOS ONLY</t>
-  </si>
-  <si>
-    <t>NIA-ALBAY CATANDUANES IRR. MGMT. OFFICE</t>
-  </si>
-  <si>
-    <t>JULY 29, 2026</t>
-  </si>
-  <si>
-    <t>JULY 29, 2025</t>
-  </si>
-  <si>
-    <t>STEPHANIE  M. RAMIREZ</t>
   </si>
   <si>
     <t>COMMONWEALTH INSURANCE COMPANY</t>
   </si>
   <si>
-    <t xml:space="preserve">               BRANCH MANAGER</t>
-  </si>
-  <si>
-    <t>Prop./Manager - DAWN ENGG. CONST. &amp; SUPPLY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ENGR. CHARLON G. CAADLAWON</t>
-  </si>
-  <si>
     <t xml:space="preserve">                    JULY 29, 2025</t>
   </si>
   <si>
-    <t>JULY 29, 2025- JULY 29, 2026</t>
+    <t>BOND NO.</t>
   </si>
   <si>
-    <t>SIX THOUSAND THREE HUNDRED</t>
+    <t>CONTRACTOR NAME - PROP ADDRESS</t>
   </si>
   <si>
-    <t>THIRTY PESOS AND 44/100 ONLY</t>
+    <t>AGENCY</t>
   </si>
   <si>
-    <t>January 9, 2025</t>
+    <t>AMOUNT IN WORDS 1</t>
   </si>
   <si>
-    <t>ANTIPOLO, BAGA,MANOC, CATANDUANES</t>
+    <t>AMOUNT IN WORDS 2</t>
   </si>
   <si>
-    <t>STEPHANIE  M. RAMIREZ - BRANCH MANAGER</t>
+    <t xml:space="preserve">COVERAGE </t>
   </si>
   <si>
-    <t>STEPHANIE M. RAMIREZ</t>
+    <t>CONTRACT NAME</t>
   </si>
   <si>
-    <t xml:space="preserve">TWO HUNDRED THIRTY FOUR THOUSAND </t>
+    <t>AMOUNT IN WORDS</t>
   </si>
   <si>
-    <t>TWO HUNDRED  PESOS ONLY</t>
+    <t>(PhpCOVERAGE; Philippine Currencies)</t>
   </si>
   <si>
-    <t>*January 9, 2025</t>
+    <t>DATE, YEAR + 1</t>
   </si>
   <si>
-    <t xml:space="preserve">          ENGR. CHARLON G. CAADLAWON</t>
+    <t>DATE, 2025</t>
+  </si>
+  <si>
+    <t>PROPIETOR</t>
+  </si>
+  <si>
+    <t>Prop./Manager - CONTRACTOR</t>
+  </si>
+  <si>
+    <t>MANAGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BRANCH MANAGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOND NO. </t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>PROPRIETOR</t>
+  </si>
+  <si>
+    <t>CTC</t>
+  </si>
+  <si>
+    <t>CTC MANAGER</t>
+  </si>
+  <si>
+    <t>CTC DATE</t>
+  </si>
+  <si>
+    <t>CTC MANAGER DATE</t>
+  </si>
+  <si>
+    <t>PROP ADDRESS</t>
+  </si>
+  <si>
+    <t>MANAGER - BRANCH MANAGER</t>
+  </si>
+  <si>
+    <t>COVERAGE</t>
+  </si>
+  <si>
+    <t>CONTRACTOR NAME</t>
+  </si>
+  <si>
+    <t>AMOUNTI N WORDS 2</t>
+  </si>
+  <si>
+    <t>RATING IN WORSD</t>
+  </si>
+  <si>
+    <t>FRACTION</t>
+  </si>
+  <si>
+    <t>RATING AMOUNT</t>
+  </si>
+  <si>
+    <t>CONTRACTOR</t>
+  </si>
+  <si>
+    <t>BOND NO;</t>
+  </si>
+  <si>
+    <t>DATE YEAR - DATE YEAR + 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -310,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -333,23 +347,19 @@
     <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -360,6 +370,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -386,7 +402,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -402,15 +417,11 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -749,11 +760,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,10 +883,10 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" s="38"/>
+      <c r="J9" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="36"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
@@ -914,7 +925,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -956,16 +967,16 @@
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
+      <c r="C16" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1012,15 +1023,15 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
+      <c r="E20" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
     </row>
     <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
@@ -1030,21 +1041,22 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
+      <c r="H21" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
     </row>
     <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="39">
-        <v>234200</v>
-      </c>
-      <c r="H22" s="38"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="36"/>
     </row>
     <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
@@ -1116,7 +1128,7 @@
     <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="5"/>
@@ -1131,14 +1143,14 @@
     <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1177,7 +1189,7 @@
     <row r="34" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="5"/>
@@ -1205,7 +1217,7 @@
     <row r="36" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="5"/>
@@ -1220,7 +1232,7 @@
     <row r="37" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="5"/>
@@ -1235,7 +1247,7 @@
     <row r="38" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="5"/>
@@ -1382,7 +1394,7 @@
       <c r="B49" s="5"/>
       <c r="C49" s="16"/>
       <c r="D49" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E49" s="17"/>
       <c r="F49" s="5"/>
@@ -1477,13 +1489,13 @@
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K56" s="5"/>
     </row>
@@ -1567,48 +1579,42 @@
     </row>
     <row r="63" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
-      <c r="C63" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D63" s="37"/>
-      <c r="E63" s="37"/>
+      <c r="B63" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
       <c r="F63" s="5"/>
-      <c r="G63" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="H63" s="55"/>
-      <c r="I63" s="55"/>
-      <c r="J63" s="55"/>
-      <c r="K63" s="55"/>
+      <c r="H63" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="52"/>
     </row>
     <row r="64" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
+      <c r="B64" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="51"/>
+      <c r="D64" s="51"/>
       <c r="F64" s="5"/>
-      <c r="G64" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="H64" s="53"/>
-      <c r="I64" s="53"/>
-      <c r="J64" s="53"/>
-      <c r="K64" s="53"/>
+      <c r="H64" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I64" s="33"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="51"/>
     </row>
     <row r="65" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
-      <c r="C65" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
+      <c r="H65" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
@@ -1634,7 +1640,7 @@
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
@@ -1657,9 +1663,6 @@
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
@@ -1670,9 +1673,6 @@
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
@@ -1683,9 +1683,6 @@
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
@@ -1745,15 +1742,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="G64:K64"/>
-    <mergeCell ref="G63:K63"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="H63:J63"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="C16:J16"/>
     <mergeCell ref="H21:K21"/>
     <mergeCell ref="E20:K20"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="H64:J64"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" horizontalDpi="120" verticalDpi="72" r:id="rId1"/>
@@ -1761,16 +1758,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L72"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:J12"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1783,7 +1780,7 @@
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -1793,15 +1790,15 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="38"/>
-    </row>
-    <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="36"/>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1813,7 +1810,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1826,23 +1823,22 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="47"/>
+      <c r="G6" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="36"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
-      <c r="L6" s="27"/>
-    </row>
-    <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -1854,9 +1850,8 @@
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
-      <c r="L7" s="27"/>
-    </row>
-    <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -1868,9 +1863,8 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="27"/>
-    </row>
-    <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -1882,74 +1876,73 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="27"/>
-    </row>
-    <row r="10" spans="1:12" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="40">
-        <v>140835</v>
-      </c>
-      <c r="F10" s="41"/>
+      <c r="E10" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="39"/>
       <c r="G10" s="10" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:12" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="22"/>
+      <c r="E11" s="21"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:12" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="50">
-        <v>1993932</v>
-      </c>
-      <c r="F12" s="50"/>
+      <c r="E12" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="47"/>
       <c r="G12" s="10" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:12" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:12" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -1962,7 +1955,7 @@
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="1:12" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -1975,7 +1968,7 @@
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="1:12" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -1988,7 +1981,7 @@
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -2001,7 +1994,7 @@
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -2014,7 +2007,7 @@
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -2027,7 +2020,7 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -2040,13 +2033,13 @@
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="38"/>
+      <c r="C21" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="36"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -2055,7 +2048,7 @@
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -2068,7 +2061,7 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -2081,7 +2074,7 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -2094,7 +2087,7 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -2107,7 +2100,7 @@
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -2120,7 +2113,7 @@
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2133,7 +2126,7 @@
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -2146,7 +2139,7 @@
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -2159,7 +2152,7 @@
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -2172,7 +2165,7 @@
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -2185,7 +2178,7 @@
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -2198,7 +2191,7 @@
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
     </row>
-    <row r="33" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -2211,7 +2204,7 @@
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -2224,10 +2217,10 @@
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
     </row>
-    <row r="35" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -2239,7 +2232,7 @@
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
     </row>
-    <row r="36" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -2252,11 +2245,11 @@
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
     </row>
-    <row r="37" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -2266,7 +2259,7 @@
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
     </row>
-    <row r="38" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -2279,7 +2272,7 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
     </row>
-    <row r="39" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -2292,7 +2285,7 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
     </row>
-    <row r="40" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -2305,7 +2298,7 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
     </row>
-    <row r="41" spans="1:11" s="25" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -2318,7 +2311,7 @@
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
     </row>
-    <row r="42" spans="1:11" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -2331,31 +2324,31 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
     </row>
-    <row r="43" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="49">
-        <v>234200</v>
-      </c>
-      <c r="G43" s="41"/>
+    <row r="43" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G43" s="39"/>
       <c r="H43" s="11"/>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
     </row>
-    <row r="44" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
+    <row r="44" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
       <c r="H44" s="10"/>
@@ -2363,7 +2356,7 @@
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
     </row>
-    <row r="45" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -2376,7 +2369,7 @@
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
-    <row r="46" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -2389,7 +2382,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
     </row>
-    <row r="47" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2402,7 +2395,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
     </row>
-    <row r="48" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -2415,7 +2408,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
     </row>
-    <row r="49" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -2428,7 +2421,7 @@
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
     </row>
-    <row r="50" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -2436,14 +2429,14 @@
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
-      <c r="H50" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="I50" s="41"/>
-      <c r="J50" s="41"/>
+      <c r="H50" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" s="39"/>
+      <c r="J50" s="39"/>
       <c r="K50" s="10"/>
     </row>
-    <row r="51" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -2456,7 +2449,7 @@
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
     </row>
-    <row r="52" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="D52" s="10"/>
@@ -2468,7 +2461,7 @@
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
@@ -2481,7 +2474,7 @@
       <c r="J53" s="10"/>
       <c r="K53" s="10"/>
     </row>
-    <row r="54" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -2494,7 +2487,7 @@
       <c r="J54" s="10"/>
       <c r="K54" s="10"/>
     </row>
-    <row r="55" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -2507,21 +2500,21 @@
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
     </row>
-    <row r="56" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
-      <c r="H56" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="I56" s="38"/>
+      <c r="H56" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I56" s="36"/>
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
     </row>
-    <row r="57" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
@@ -2533,7 +2526,7 @@
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
     </row>
-    <row r="58" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -2542,120 +2535,120 @@
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
-      <c r="J58" s="44">
-        <v>1993932</v>
-      </c>
-      <c r="K58" s="44"/>
-    </row>
-    <row r="59" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="44"/>
-      <c r="C59" s="41"/>
+      <c r="J58" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="K58" s="42"/>
+    </row>
+    <row r="59" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="42"/>
+      <c r="C59" s="39"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
       <c r="H59" s="12" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="I59" s="8"/>
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
     </row>
-    <row r="60" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:11" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:11" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:11" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:11" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:11" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="21"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="21"/>
-      <c r="H65" s="21"/>
-      <c r="I65" s="21"/>
-      <c r="J65" s="21"/>
-      <c r="K65" s="21"/>
+      <c r="A65" s="20"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
     </row>
     <row r="66" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="21"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="21"/>
-      <c r="H66" s="21"/>
-      <c r="I66" s="21"/>
-      <c r="J66" s="21"/>
-      <c r="K66" s="21"/>
+      <c r="A66" s="20"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
     </row>
     <row r="67" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="21"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="21"/>
-      <c r="H67" s="21"/>
-      <c r="I67" s="21"/>
-      <c r="J67" s="21"/>
-      <c r="K67" s="21"/>
+      <c r="A67" s="20"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="20"/>
+      <c r="I67" s="20"/>
+      <c r="J67" s="20"/>
+      <c r="K67" s="20"/>
     </row>
     <row r="68" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="21"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="21"/>
-      <c r="H68" s="21"/>
-      <c r="I68" s="21"/>
-      <c r="J68" s="21"/>
-      <c r="K68" s="21"/>
+      <c r="A68" s="20"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="20"/>
+      <c r="I68" s="20"/>
+      <c r="J68" s="20"/>
+      <c r="K68" s="20"/>
     </row>
     <row r="69" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="21"/>
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="21"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="21"/>
+      <c r="A69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="20"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="20"/>
+      <c r="K69" s="20"/>
     </row>
     <row r="70" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="21"/>
-      <c r="H70" s="21"/>
-      <c r="I70" s="21"/>
-      <c r="J70" s="21"/>
-      <c r="K70" s="21"/>
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
     </row>
     <row r="71" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="21"/>
-      <c r="B71" s="21"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="21"/>
-      <c r="H71" s="21"/>
-      <c r="I71" s="21"/>
-      <c r="J71" s="21"/>
-      <c r="K71" s="21"/>
+      <c r="A71" s="20"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="20"/>
+      <c r="I71" s="20"/>
+      <c r="J71" s="20"/>
+      <c r="K71" s="20"/>
     </row>
     <row r="72" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2679,16 +2672,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F25" sqref="F25:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2698,12 +2691,12 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="38"/>
-    </row>
-    <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="36"/>
+    </row>
+    <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2716,7 +2709,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -2729,7 +2722,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2742,7 +2735,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2755,7 +2748,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2768,7 +2761,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -2781,7 +2774,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2794,7 +2787,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2807,7 +2800,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2820,7 +2813,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2832,10 +2825,8 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-    </row>
-    <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2847,10 +2838,8 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-    </row>
-    <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2862,10 +2851,8 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-    </row>
-    <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2877,10 +2864,8 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-    </row>
-    <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2892,10 +2877,8 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-    </row>
-    <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2907,62 +2890,45 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-    </row>
-    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
+    </row>
+    <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
+        <v>36</v>
+      </c>
       <c r="F17" s="5"/>
-      <c r="G17" s="51" t="s">
+      <c r="G17" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-    </row>
-    <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="52">
-        <v>234200</v>
-      </c>
-      <c r="G18" s="47"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+    </row>
+    <row r="18" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="36"/>
       <c r="H18" s="2"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-    </row>
-    <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
+    </row>
+    <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
+        <v>13</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-    </row>
-    <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2974,10 +2940,8 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-    </row>
-    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2989,10 +2953,8 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-    </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -3004,10 +2966,8 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-    </row>
-    <row r="23" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -3019,46 +2979,40 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-    </row>
-    <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-    </row>
-    <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+    </row>
+    <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="7" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="52">
-        <v>4226.4960000000001</v>
-      </c>
-      <c r="G25" s="47"/>
+      <c r="F25" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="36"/>
       <c r="H25" s="2"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-    </row>
-    <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -3066,16 +3020,14 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-    </row>
-    <row r="27" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -3087,10 +3039,8 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-    </row>
-    <row r="28" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -3102,10 +3052,8 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-    </row>
-    <row r="29" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -3117,10 +3065,8 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-    </row>
-    <row r="30" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -3132,10 +3078,8 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-    </row>
-    <row r="31" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -3148,7 +3092,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3210,11 +3154,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3466,7 +3410,7 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -3522,7 +3466,7 @@
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -3536,16 +3480,16 @@
     <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
-      <c r="C25" s="21"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="21"/>
+      <c r="E25" s="20"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="J25" s="38"/>
+      <c r="I25" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" s="36"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3564,14 +3508,14 @@
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="9" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="8" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
@@ -3580,7 +3524,7 @@
     <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -3776,7 +3720,7 @@
     <row r="43" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -3809,10 +3753,10 @@
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="I45" s="38"/>
+      <c r="H45" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I45" s="36"/>
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
     </row>
@@ -3910,14 +3854,14 @@
     <row r="53" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="6" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
@@ -4031,21 +3975,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -4056,7 +4000,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="21"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
@@ -4068,7 +4012,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="21"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
@@ -4080,7 +4024,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="21"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
@@ -4092,37 +4036,39 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="21"/>
+      <c r="H4" s="20"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="21"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="B6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="21"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7"/>
@@ -4130,23 +4076,23 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="21"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="21"/>
+      <c r="H8" s="20"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -4155,49 +4101,49 @@
       <c r="F9" s="7"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="24"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="7"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="24"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="7"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="31"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="32">
+      <c r="E13" s="28" t="e">
         <f>E30</f>
-        <v>6330.4405120000001</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -4206,169 +4152,169 @@
       <c r="F14" s="7"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="41"/>
+      <c r="B15" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="39"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C16" s="7"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="E17" s="24">
-        <v>4226.4960000000001</v>
+      <c r="E17" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="32">
+      <c r="E18" s="28" t="e">
         <f>12.5%*E17</f>
-        <v>528.31200000000001</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="14"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="24"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="7"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="24"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="7"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
-      <c r="E21" s="32">
+      <c r="E21" s="28" t="e">
         <f>0.2%*E17</f>
-        <v>8.4529920000000001</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="15"/>
       <c r="C22" s="7"/>
-      <c r="E22" s="24">
+      <c r="E22" s="23">
         <v>1060</v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="41"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="39"/>
       <c r="F23" s="7"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="E24" s="32">
+      <c r="E24" s="28" t="e">
         <f>12%*E17</f>
-        <v>507.17951999999997</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="4"/>
       <c r="C25" s="7"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="32">
+      <c r="E27" s="28" t="e">
         <f>SUM(E17:E24)</f>
-        <v>6330.4405120000001</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="20" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="33">
+      <c r="B28" s="29" t="str">
         <f>E17</f>
-        <v>4226.4960000000001</v>
+        <v>RATING AMOUNT</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="34"/>
+      <c r="D28" s="30"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="35"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="35">
+      <c r="B30" s="31">
         <f>D23</f>
         <v>0</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="36">
+      <c r="E30" s="32" t="e">
         <f>E27</f>
-        <v>6330.4405120000001</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="35"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="31"/>
+      <c r="E31" s="27"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="35">
+      <c r="B32" s="31">
         <f>D25</f>
         <v>0</v>
       </c>
@@ -4378,9 +4324,9 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="24">
+      <c r="B33" s="23">
         <f>D30</f>
         <v>0</v>
       </c>
@@ -4398,7 +4344,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="21"/>
+      <c r="H34" s="20"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
@@ -4410,7 +4356,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="21"/>
+      <c r="H35" s="20"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
@@ -4439,27 +4385,27 @@
       <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
       <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
       <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>